<commit_message>
I have created a template for the project
</commit_message>
<xml_diff>
--- a/End_year/Resources/ER_Database.xlsx
+++ b/End_year/Resources/ER_Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t xml:space="preserve">Database</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">Will be a string, Password to be max 10 characters long</t>
   </si>
   <si>
+    <t xml:space="preserve">Maybe we store hashed passwords here</t>
+  </si>
+  <si>
     <t xml:space="preserve">products</t>
   </si>
   <si>
@@ -85,23 +88,7 @@
     <t xml:space="preserve">product_specs</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Will be a JSON object, of strings </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{”spec_name”:”spec_detail”, ”spec_name”:”spec_detail”}</t>
-    </r>
+    <t xml:space="preserve">Will be a JSON object, of strings {”spec_name”:”spec_detail”, ”spec_name”:”spec_detail”}</t>
   </si>
   <si>
     <t xml:space="preserve">user_details</t>
@@ -144,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -186,11 +173,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -357,16 +339,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.82"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,79 +397,82 @@
       <c r="B10" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C10" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,92 +480,92 @@
         <v>6</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust database and added the data parsing table
</commit_message>
<xml_diff>
--- a/End_year/Resources/ER_Database.xlsx
+++ b/End_year/Resources/ER_Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t xml:space="preserve">Database</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">Maybe we store hashed passwords here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logged_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be a boolean, 0 or 1</t>
   </si>
   <si>
     <t xml:space="preserve">products</t>
@@ -339,16 +345,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.82"/>
   </cols>
   <sheetData>
@@ -401,49 +407,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,121 +457,129 @@
         <v>19</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="B24" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>31</v>
+      <c r="A31" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>33</v>
+      <c r="A34" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>